<commit_message>
Cenários finalizados em Junit
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinset/HUB_TDD/TestData/TestData.xlsx
+++ b/src/test/java/br/com/rsinset/HUB_TDD/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.costa\eclipse-workspace\servlets\HUB_TDD\src\test\java\br\com\rsinset\HUB_TDD\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086D0249-05EE-4F52-B425-DEEF2F73332A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270D0615-57CC-4202-B8C5-3DD5106D3DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A238A30-1AA3-4A42-BD5B-6DAF71D155B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A238A30-1AA3-4A42-BD5B-6DAF71D155B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>email</t>
   </si>
@@ -66,27 +66,6 @@
     <t>cep</t>
   </si>
   <si>
-    <t>pedro999</t>
-  </si>
-  <si>
-    <t>pedro999@email.com</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>Alves Melo</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Lisboa</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro</t>
-  </si>
-  <si>
     <t>usuario</t>
   </si>
   <si>
@@ -96,9 +75,6 @@
     <t>João</t>
   </si>
   <si>
-    <t>*Pedro999</t>
-  </si>
-  <si>
     <t>*Joao123</t>
   </si>
   <si>
@@ -114,24 +90,12 @@
     <t>Av. Paulista, 200</t>
   </si>
   <si>
-    <t>Av. Brasil, 1000</t>
-  </si>
-  <si>
     <t>01311-922</t>
   </si>
   <si>
     <t>1198888-8888</t>
   </si>
   <si>
-    <t>1196677-8899</t>
-  </si>
-  <si>
-    <t>5599-055</t>
-  </si>
-  <si>
-    <t>joao126</t>
-  </si>
-  <si>
     <t>HP ROAR WIRELESS SPEAKER</t>
   </si>
   <si>
@@ -142,14 +106,25 @@
   </si>
   <si>
     <t>mouse gamer</t>
+  </si>
+  <si>
+    <t>joao1211</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -165,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -173,13 +148,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +563,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,134 +580,100 @@
     <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conversão para TestNG e adição do report
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinset/HUB_TDD/TestData/TestData.xlsx
+++ b/src/test/java/br/com/rsinset/HUB_TDD/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.costa\eclipse-workspace\servlets\HUB_TDD\src\test\java\br\com\rsinset\HUB_TDD\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270D0615-57CC-4202-B8C5-3DD5106D3DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E53B7A-9343-49DB-A391-7D11C7BA9C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A238A30-1AA3-4A42-BD5B-6DAF71D155B8}"/>
   </bookViews>
@@ -108,7 +108,7 @@
     <t>mouse gamer</t>
   </si>
   <si>
-    <t>joao1211</t>
+    <t>joao12366</t>
   </si>
 </sst>
 </file>
@@ -140,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -198,19 +198,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -241,11 +228,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +556,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,40 +574,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -661,10 +654,10 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>